<commit_message>
improve framework remove status webdriver
</commit_message>
<xml_diff>
--- a/testData/Opencart_LoginData.xlsx
+++ b/testData/Opencart_LoginData.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-105" yWindow="225" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>username</t>
   </si>
@@ -63,9 +63,6 @@
     <t>xyz</t>
   </si>
   <si>
-    <t>pavanoltraining@gmail.com</t>
-  </si>
-  <si>
     <t>test@123</t>
   </si>
   <si>
@@ -79,6 +76,12 @@
   </si>
   <si>
     <t>inValid</t>
+  </si>
+  <si>
+    <t>tejaszombade55@gmail.com</t>
+  </si>
+  <si>
+    <t>Tztejas@13</t>
   </si>
 </sst>
 </file>
@@ -497,7 +500,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,15 +521,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="20.65" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
+    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="20.65" x14ac:dyDescent="0.55000000000000004">
@@ -564,10 +567,10 @@
     </row>
     <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>5</v>
@@ -575,10 +578,10 @@
     </row>
     <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>15</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>5</v>

</xml_diff>